<commit_message>
added new window for the items
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/Orders/OrderData.xlsx
+++ b/Group14-A2/src/main/java/Orders/OrderData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>Order ID</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>dineIn</t>
+  </si>
+  <si>
+    <t>[2, 2, 2, 2, 2, 2]</t>
   </si>
 </sst>
 </file>
@@ -95,7 +98,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -229,6 +232,26 @@
         <v>3.0</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
added new feature for the waiter order
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/Orders/OrderData.xlsx
+++ b/Group14-A2/src/main/java/Orders/OrderData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\javafx-restaurant-app\Group14-A2\src\main\java\Orders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6996A2F-544F-4C3D-892B-AC0DA422D27C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005DD0E8-8E36-4835-A5A1-F8C49CD5CADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Order ID</t>
   </si>
@@ -56,6 +56,18 @@
   </si>
   <si>
     <t>Cancelled</t>
+  </si>
+  <si>
+    <t>Waiter ID</t>
+  </si>
+  <si>
+    <t>Chef ID</t>
+  </si>
+  <si>
+    <t>Driver ID</t>
+  </si>
+  <si>
+    <t>[1, 1, 1, 2, 2, 2]</t>
   </si>
 </sst>
 </file>
@@ -408,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -424,7 +436,7 @@
     <col min="6" max="6" bestFit="true" customWidth="true" width="12.1484375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -443,10 +455,19 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1.0</v>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -460,13 +481,22 @@
       <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="n">
-        <v>4.0</v>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2.0</v>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -480,13 +510,22 @@
       <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="n">
-        <v>4.0</v>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3.0</v>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -500,8 +539,46 @@
       <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
         <v>4.0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed feature for the order page for waiter
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/Orders/OrderData.xlsx
+++ b/Group14-A2/src/main/java/Orders/OrderData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>Order ID</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>[1, 1, 1, 2, 2, 2]</t>
+  </si>
+  <si>
+    <t>[2, 2, 2, 2, 3]</t>
   </si>
 </sst>
 </file>
@@ -420,7 +423,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L8" sqref="L8"/>
@@ -581,6 +584,35 @@
         <v>0.0</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fininshed the functionality for waiter order section
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/Orders/OrderData.xlsx
+++ b/Group14-A2/src/main/java/Orders/OrderData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\javafx-restaurant-app\Group14-A2\src\main\java\Orders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005DD0E8-8E36-4835-A5A1-F8C49CD5CADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D2BB53-A446-4304-932D-3FDB0FB920A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Order Data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>Order ID</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>[2, 2, 2, 2, 3]</t>
+  </si>
+  <si>
+    <t>Completed</t>
   </si>
 </sst>
 </file>
@@ -425,18 +428,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.68359375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.09375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="31.59765625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="22.66015625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.1796875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.1484375" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.6640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="31.5546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="22.6640625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.21875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -479,16 +482,16 @@
         <v>7</v>
       </c>
       <c r="D2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F2">
         <v>4</v>
       </c>
-      <c r="G2">
-        <v>0</v>
+      <c r="G2" t="n">
+        <v>7.0</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -555,9 +558,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4.0</v>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -571,22 +574,22 @@
       <c r="E5" t="s">
         <v>8</v>
       </c>
-      <c r="F5" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.0</v>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5.0</v>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -595,22 +598,22 @@
         <v>16</v>
       </c>
       <c r="D6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.0</v>
+        <v>17</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
       </c>
       <c r="G6" t="n">
         <v>7.0</v>
       </c>
-      <c r="H6" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.0</v>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed a bug causing issues in the waiter add order
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/Orders/OrderData.xlsx
+++ b/Group14-A2/src/main/java/Orders/OrderData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
   <si>
     <t>Order ID</t>
   </si>
@@ -74,6 +74,18 @@
   </si>
   <si>
     <t>Completed</t>
+  </si>
+  <si>
+    <t>[1, 1, 2, 2]</t>
+  </si>
+  <si>
+    <t>[2, 2, 2]</t>
+  </si>
+  <si>
+    <t>[7, 7, 5]</t>
+  </si>
+  <si>
+    <t>[1, 1, 4]</t>
   </si>
 </sst>
 </file>
@@ -426,7 +438,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
@@ -434,12 +446,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.6640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="31.5546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="22.6640625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.21875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.109375" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.68359375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.09375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="31.59765625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="22.66015625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.1796875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.1484375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -616,6 +628,122 @@
         <v>0</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added jdocs in 2 files
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/Orders/OrderData.xlsx
+++ b/Group14-A2/src/main/java/Orders/OrderData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
   <si>
     <t>Order ID</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>[1, 1, 4]</t>
+  </si>
+  <si>
+    <t>[1, 2, 2]</t>
   </si>
 </sst>
 </file>
@@ -438,7 +441,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
@@ -744,6 +747,35 @@
         <v>0.0</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed issue where the page does not load
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/Orders/OrderData.xlsx
+++ b/Group14-A2/src/main/java/Orders/OrderData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\javafx-restaurant-app\Group14-A2\src\main\java\Orders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D2BB53-A446-4304-932D-3FDB0FB920A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E752DC6-5AE7-443A-8850-C16DA3E9F739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Order Data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
   <si>
     <t>Order ID</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>[1, 2, 2]</t>
+  </si>
+  <si>
+    <t>Food Prepared</t>
   </si>
 </sst>
 </file>
@@ -443,18 +446,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.68359375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.09375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="31.59765625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="22.66015625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.1796875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.1484375" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.6640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="31.5546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="22.6640625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.21875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -505,8 +508,8 @@
       <c r="F2">
         <v>4</v>
       </c>
-      <c r="G2" t="n">
-        <v>7.0</v>
+      <c r="G2">
+        <v>7</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -555,10 +558,10 @@
         <v>10</v>
       </c>
       <c r="D4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="F4">
         <v>4</v>
@@ -567,7 +570,7 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -584,10 +587,10 @@
         <v>15</v>
       </c>
       <c r="D5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -595,8 +598,8 @@
       <c r="G5">
         <v>0</v>
       </c>
-      <c r="H5">
-        <v>0</v>
+      <c r="H5" t="n">
+        <v>5.0</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -621,8 +624,8 @@
       <c r="F6">
         <v>0</v>
       </c>
-      <c r="G6" t="n">
-        <v>7.0</v>
+      <c r="G6">
+        <v>7</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -631,9 +634,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6.0</v>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -647,22 +650,22 @@
       <c r="E7" t="s">
         <v>8</v>
       </c>
-      <c r="F7" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G7" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7.0</v>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>7</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -671,27 +674,27 @@
         <v>19</v>
       </c>
       <c r="D8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>7</v>
+      </c>
+      <c r="H8" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9">
         <v>8</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G8" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8.0</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -705,22 +708,22 @@
       <c r="E9" t="s">
         <v>8</v>
       </c>
-      <c r="F9" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G9" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9.0</v>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>7</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -734,22 +737,22 @@
       <c r="E10" t="s">
         <v>8</v>
       </c>
-      <c r="F10" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G10" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10.0</v>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>7</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -763,17 +766,17 @@
       <c r="E11" t="s">
         <v>8</v>
       </c>
-      <c r="F11" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0.0</v>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed the driver part
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/Orders/OrderData.xlsx
+++ b/Group14-A2/src/main/java/Orders/OrderData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\javafx-restaurant-app\Group14-A2\src\main\java\Orders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E752DC6-5AE7-443A-8850-C16DA3E9F739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C47318-FE38-4BEF-BD48-4D3F3A7C6937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
   <si>
     <t>Order ID</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>Food Prepared</t>
+  </si>
+  <si>
+    <t>Delivery</t>
   </si>
 </sst>
 </file>
@@ -447,7 +450,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -561,7 +564,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F4">
         <v>4</v>
@@ -572,8 +575,8 @@
       <c r="H4">
         <v>5</v>
       </c>
-      <c r="I4">
-        <v>0</v>
+      <c r="I4" t="n">
+        <v>8.0</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -590,7 +593,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -598,11 +601,11 @@
       <c r="G5">
         <v>0</v>
       </c>
-      <c r="H5" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5" t="n">
+        <v>8.0</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -685,8 +688,8 @@
       <c r="G8">
         <v>7</v>
       </c>
-      <c r="H8" t="n">
-        <v>5.0</v>
+      <c r="H8">
+        <v>5</v>
       </c>
       <c r="I8">
         <v>0</v>

</xml_diff>

<commit_message>
added css to the whole customer file
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/Orders/OrderData.xlsx
+++ b/Group14-A2/src/main/java/Orders/OrderData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
   <si>
     <t>Order ID</t>
   </si>
@@ -95,6 +95,12 @@
   </si>
   <si>
     <t>Delivery</t>
+  </si>
+  <si>
+    <t>delivery</t>
+  </si>
+  <si>
+    <t>[4]</t>
   </si>
 </sst>
 </file>
@@ -447,7 +453,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
@@ -455,12 +461,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.6640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="31.5546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="22.6640625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.21875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.109375" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.68359375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.09375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="31.59765625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="22.66015625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.24609375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.1484375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -782,6 +788,35 @@
         <v>0</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added css to the customer page
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/Orders/OrderData.xlsx
+++ b/Group14-A2/src/main/java/Orders/OrderData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
   <si>
     <t>Order ID</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>[4]</t>
+  </si>
+  <si>
+    <t>[4, 4, 6, 3, 3, 2]</t>
   </si>
 </sst>
 </file>
@@ -453,7 +456,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
@@ -817,6 +820,35 @@
         <v>0.0</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added styling to driver [age
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/Orders/OrderData.xlsx
+++ b/Group14-A2/src/main/java/Orders/OrderData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\javafx-restaurant-app\Group14-A2\src\main\java\Orders\"/>
     </mc:Choice>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
   <si>
     <t>Order ID</t>
   </si>
@@ -110,12 +110,16 @@
   </si>
   <si>
     <t>[1]</t>
+  </si>
+  <si>
+    <t>Delivery</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -469,12 +473,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="31.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.6640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="31.5546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="22.6640625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.21875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -926,7 +930,7 @@
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="F16">
         <v>4</v>
@@ -937,8 +941,8 @@
       <c r="H16">
         <v>0</v>
       </c>
-      <c r="I16">
-        <v>0</v>
+      <c r="I16" t="n">
+        <v>8.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>